<commit_message>
update evaluation for noun
</commit_message>
<xml_diff>
--- a/Evaluation/Annotated_files/annotated_evaluation_results_npee_mc_SFT_only.xlsx
+++ b/Evaluation/Annotated_files/annotated_evaluation_results_npee_mc_SFT_only.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annica\PycharmProjects\master_thesis\Evaluation\Annotated_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC3158C-59A5-49B4-8766-EE1FE594A738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="10780" windowHeight="15370" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="evaluation_results_npee_closed_" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="evaluation_results_npee_closed_" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -22,22 +38,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="182">
   <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">input</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pred</t>
-  </si>
-  <si>
-    <t xml:space="preserve">evaluation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>pred</t>
+  </si>
+  <si>
+    <t>evaluation</t>
+  </si>
+  <si>
+    <t>choice</t>
   </si>
   <si>
     <t xml:space="preserve"> 
@@ -48,7 +64,7 @@
 C. Wave marks, mud cracks, parallel bedding </t>
   </si>
   <si>
-    <t xml:space="preserve">C</t>
+    <t>C</t>
   </si>
   <si>
     <t xml:space="preserve"> #B  </t>
@@ -79,7 +95,7 @@
 D. Stone Salt Pseudocrystal </t>
   </si>
   <si>
-    <t xml:space="preserve">B</t>
+    <t>B</t>
   </si>
   <si>
     <t xml:space="preserve"> 
@@ -91,7 +107,7 @@
 D. Joint </t>
   </si>
   <si>
-    <t xml:space="preserve">D</t>
+    <t>D</t>
   </si>
   <si>
     <t xml:space="preserve"> #B 
@@ -353,7 +369,7 @@
 D. Dynamic metamorphism </t>
   </si>
   <si>
-    <t xml:space="preserve">A</t>
+    <t>A</t>
   </si>
   <si>
     <t xml:space="preserve"> 
@@ -1131,7 +1147,7 @@
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">＋</t>
+      <t>＋</t>
     </r>
     <r>
       <rPr>
@@ -1139,7 +1155,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">: Fe2</t>
+      <t>: Fe2</t>
     </r>
     <r>
       <rPr>
@@ -1455,21 +1471,20 @@
     <t xml:space="preserve"> #D. cataclastic  </t>
   </si>
   <si>
-    <t xml:space="preserve">Sum of all correct answers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average of correct answers in %</t>
+    <t>Sum of all correct answers</t>
+  </si>
+  <si>
+    <t>Average of correct answers in %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00\ %"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00\ %"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1477,35 +1492,26 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1513,107 +1519,88 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18a303"/>
+        <a:srgbClr val="18A303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369a3"/>
+        <a:srgbClr val="0369A3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a33e03"/>
+        <a:srgbClr val="A33E03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8e03a3"/>
+        <a:srgbClr val="8E03A3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="c99c00"/>
+        <a:srgbClr val="C99C00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="c9211e"/>
+        <a:srgbClr val="C9211E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ee"/>
+        <a:srgbClr val="0000EE"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551a8b"/>
+        <a:srgbClr val="551A8B"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -1666,31 +1653,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A181" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D188" activeCellId="0" sqref="D188"/>
+    <sheetView tabSelected="1" topLeftCell="C183" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D184" sqref="D184:E185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="30.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="53.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.64"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="6" style="1" width="30.65"/>
+    <col min="1" max="1" width="13.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="43.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="1" customWidth="1"/>
+    <col min="4" max="4" width="53.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="30.6328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1707,7 +1693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="167.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1720,11 +1706,11 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1737,11 +1723,11 @@
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1754,11 +1740,11 @@
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1771,11 +1757,11 @@
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1788,11 +1774,11 @@
       <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1805,11 +1791,11 @@
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="211.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="137.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1822,11 +1808,11 @@
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1839,11 +1825,11 @@
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1856,11 +1842,11 @@
       <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1873,11 +1859,11 @@
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="156.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1890,11 +1876,11 @@
       <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1907,11 +1893,11 @@
       <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1924,11 +1910,11 @@
       <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1941,11 +1927,11 @@
       <c r="D15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1958,11 +1944,11 @@
       <c r="D16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -1975,11 +1961,11 @@
       <c r="D17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="79" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1992,11 +1978,11 @@
       <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -2009,11 +1995,11 @@
       <c r="D19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -2026,11 +2012,11 @@
       <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -2043,11 +2029,11 @@
       <c r="D21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="79" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -2060,11 +2046,11 @@
       <c r="D22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
@@ -2077,11 +2063,11 @@
       <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -2094,11 +2080,11 @@
       <c r="D24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -2111,11 +2097,11 @@
       <c r="D25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
@@ -2128,11 +2114,11 @@
       <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -2145,11 +2131,11 @@
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -2162,11 +2148,11 @@
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -2179,11 +2165,11 @@
       <c r="D29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="178.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -2196,11 +2182,11 @@
       <c r="D30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="277.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
@@ -2213,11 +2199,11 @@
       <c r="D31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -2230,11 +2216,11 @@
       <c r="D32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
@@ -2247,11 +2233,11 @@
       <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="156.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -2264,11 +2250,11 @@
       <c r="D34" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
@@ -2281,11 +2267,11 @@
       <c r="D35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
@@ -2298,11 +2284,11 @@
       <c r="D36" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="156.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
@@ -2315,11 +2301,11 @@
       <c r="D37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E37" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
@@ -2332,11 +2318,11 @@
       <c r="D38" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E38" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="156.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
@@ -2349,11 +2335,11 @@
       <c r="D39" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
@@ -2366,11 +2352,11 @@
       <c r="D40" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
@@ -2383,11 +2369,11 @@
       <c r="D41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
@@ -2400,11 +2386,11 @@
       <c r="D42" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E42" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
@@ -2417,11 +2403,11 @@
       <c r="D43" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E43" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
@@ -2434,11 +2420,11 @@
       <c r="D44" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="167.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
@@ -2451,11 +2437,11 @@
       <c r="D45" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E45" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>5</v>
       </c>
@@ -2468,11 +2454,11 @@
       <c r="D46" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E46" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>5</v>
       </c>
@@ -2485,11 +2471,11 @@
       <c r="D47" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E47" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
@@ -2502,11 +2488,11 @@
       <c r="D48" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E48" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
@@ -2519,11 +2505,11 @@
       <c r="D49" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
@@ -2536,11 +2522,11 @@
       <c r="D50" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E50" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
@@ -2553,11 +2539,11 @@
       <c r="D51" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E51" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
@@ -2570,11 +2556,11 @@
       <c r="D52" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>5</v>
       </c>
@@ -2587,11 +2573,11 @@
       <c r="D53" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
@@ -2604,11 +2590,11 @@
       <c r="D54" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E54" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="200.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>5</v>
       </c>
@@ -2621,11 +2607,11 @@
       <c r="D55" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E55" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>5</v>
       </c>
@@ -2638,11 +2624,11 @@
       <c r="D56" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E56" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>5</v>
       </c>
@@ -2655,11 +2641,11 @@
       <c r="D57" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E57" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>5</v>
       </c>
@@ -2672,11 +2658,11 @@
       <c r="D58" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E58" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>5</v>
       </c>
@@ -2689,11 +2675,11 @@
       <c r="D59" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E59" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="189.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="137.5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>5</v>
       </c>
@@ -2706,11 +2692,11 @@
       <c r="D60" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E60" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>5</v>
       </c>
@@ -2723,11 +2709,11 @@
       <c r="D61" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E61" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>5</v>
       </c>
@@ -2740,11 +2726,11 @@
       <c r="D62" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E62" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
@@ -2757,11 +2743,11 @@
       <c r="D63" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E63" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
@@ -2774,11 +2760,11 @@
       <c r="D64" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E64" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="200.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="137.5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
@@ -2791,11 +2777,11 @@
       <c r="D65" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E65" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>5</v>
       </c>
@@ -2808,11 +2794,11 @@
       <c r="D66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E66" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
@@ -2825,11 +2811,11 @@
       <c r="D67" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E67" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E67" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>5</v>
       </c>
@@ -2842,11 +2828,11 @@
       <c r="D68" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E68" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>5</v>
       </c>
@@ -2859,11 +2845,11 @@
       <c r="D69" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E69" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E69" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -2876,11 +2862,11 @@
       <c r="D70" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E70" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
@@ -2893,11 +2879,11 @@
       <c r="D71" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
@@ -2910,11 +2896,11 @@
       <c r="D72" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E72" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>5</v>
       </c>
@@ -2927,11 +2913,11 @@
       <c r="D73" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E73" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>5</v>
       </c>
@@ -2944,11 +2930,11 @@
       <c r="D74" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E74" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E74" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>5</v>
       </c>
@@ -2961,11 +2947,11 @@
       <c r="D75" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E75" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E75" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>5</v>
       </c>
@@ -2978,11 +2964,11 @@
       <c r="D76" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E76" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>5</v>
       </c>
@@ -2995,11 +2981,11 @@
       <c r="D77" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E77" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>5</v>
       </c>
@@ -3012,11 +2998,11 @@
       <c r="D78" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E78" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E78" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>5</v>
       </c>
@@ -3029,11 +3015,11 @@
       <c r="D79" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E79" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="178.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>5</v>
       </c>
@@ -3046,11 +3032,11 @@
       <c r="D80" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E80" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="277.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>5</v>
       </c>
@@ -3063,11 +3049,11 @@
       <c r="D81" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E81" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>5</v>
       </c>
@@ -3080,11 +3066,11 @@
       <c r="D82" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E82" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E82" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>5</v>
       </c>
@@ -3097,11 +3083,11 @@
       <c r="D83" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E83" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="156.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>5</v>
       </c>
@@ -3114,11 +3100,11 @@
       <c r="D84" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E84" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E84" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>5</v>
       </c>
@@ -3131,11 +3117,11 @@
       <c r="D85" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E85" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E85" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>5</v>
       </c>
@@ -3148,11 +3134,11 @@
       <c r="D86" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E86" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E86" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>5</v>
       </c>
@@ -3165,11 +3151,11 @@
       <c r="D87" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E87" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="156.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E87" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>5</v>
       </c>
@@ -3182,11 +3168,11 @@
       <c r="D88" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E88" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>5</v>
       </c>
@@ -3199,11 +3185,11 @@
       <c r="D89" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E89" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E89" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>5</v>
       </c>
@@ -3216,11 +3202,11 @@
       <c r="D90" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E90" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E90" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>5</v>
       </c>
@@ -3233,11 +3219,11 @@
       <c r="D91" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E91" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E91" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>5</v>
       </c>
@@ -3250,11 +3236,11 @@
       <c r="D92" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E92" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>5</v>
       </c>
@@ -3267,11 +3253,11 @@
       <c r="D93" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E93" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E93" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>5</v>
       </c>
@@ -3284,11 +3270,11 @@
       <c r="D94" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E94" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E94" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>5</v>
       </c>
@@ -3301,11 +3287,11 @@
       <c r="D95" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E95" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E95" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>5</v>
       </c>
@@ -3318,11 +3304,11 @@
       <c r="D96" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E96" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E96" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>5</v>
       </c>
@@ -3335,11 +3321,11 @@
       <c r="D97" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E97" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="200.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>5</v>
       </c>
@@ -3352,11 +3338,11 @@
       <c r="D98" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E98" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>5</v>
       </c>
@@ -3369,11 +3355,11 @@
       <c r="D99" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E99" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>5</v>
       </c>
@@ -3386,11 +3372,11 @@
       <c r="D100" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E100" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>5</v>
       </c>
@@ -3403,11 +3389,11 @@
       <c r="D101" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E101" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E101" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>5</v>
       </c>
@@ -3420,11 +3406,11 @@
       <c r="D102" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E102" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="189.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="137.5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>5</v>
       </c>
@@ -3437,11 +3423,11 @@
       <c r="D103" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E103" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E103" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>5</v>
       </c>
@@ -3454,11 +3440,11 @@
       <c r="D104" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E104" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E104" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>5</v>
       </c>
@@ -3471,11 +3457,11 @@
       <c r="D105" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E105" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E105" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>5</v>
       </c>
@@ -3488,11 +3474,11 @@
       <c r="D106" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E106" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E106" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>5</v>
       </c>
@@ -3505,11 +3491,11 @@
       <c r="D107" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E107" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="200.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E107" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="137.5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>5</v>
       </c>
@@ -3522,11 +3508,11 @@
       <c r="D108" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E108" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E108" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>5</v>
       </c>
@@ -3539,11 +3525,11 @@
       <c r="D109" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E109" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E109" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>5</v>
       </c>
@@ -3556,11 +3542,11 @@
       <c r="D110" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E110" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E110" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>5</v>
       </c>
@@ -3573,11 +3559,11 @@
       <c r="D111" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E111" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E111" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>5</v>
       </c>
@@ -3590,11 +3576,11 @@
       <c r="D112" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E112" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E112" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>5</v>
       </c>
@@ -3607,11 +3593,11 @@
       <c r="D113" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E113" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E113" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>5</v>
       </c>
@@ -3624,11 +3610,11 @@
       <c r="D114" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E114" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>5</v>
       </c>
@@ -3641,11 +3627,11 @@
       <c r="D115" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E115" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E115" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>5</v>
       </c>
@@ -3658,11 +3644,11 @@
       <c r="D116" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E116" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E116" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>5</v>
       </c>
@@ -3675,11 +3661,11 @@
       <c r="D117" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E117" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E117" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>5</v>
       </c>
@@ -3692,11 +3678,11 @@
       <c r="D118" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E118" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E118" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>5</v>
       </c>
@@ -3709,11 +3695,11 @@
       <c r="D119" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E119" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E119" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>5</v>
       </c>
@@ -3726,11 +3712,11 @@
       <c r="D120" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E120" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E120" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>5</v>
       </c>
@@ -3743,11 +3729,11 @@
       <c r="D121" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E121" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E121" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>5</v>
       </c>
@@ -3760,11 +3746,11 @@
       <c r="D122" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E122" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E122" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>5</v>
       </c>
@@ -3777,11 +3763,11 @@
       <c r="D123" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E123" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E123" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>5</v>
       </c>
@@ -3794,11 +3780,11 @@
       <c r="D124" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E124" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E124" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>5</v>
       </c>
@@ -3811,11 +3797,11 @@
       <c r="D125" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E125" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E125" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>5</v>
       </c>
@@ -3828,11 +3814,11 @@
       <c r="D126" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E126" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E126" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>5</v>
       </c>
@@ -3845,11 +3831,11 @@
       <c r="D127" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E127" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E127" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>5</v>
       </c>
@@ -3862,11 +3848,11 @@
       <c r="D128" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E128" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="200.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E128" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="137.5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>5</v>
       </c>
@@ -3879,11 +3865,11 @@
       <c r="D129" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E129" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E129" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>5</v>
       </c>
@@ -3896,11 +3882,11 @@
       <c r="D130" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E130" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E130" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>5</v>
       </c>
@@ -3913,11 +3899,11 @@
       <c r="D131" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E131" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E131" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>5</v>
       </c>
@@ -3930,11 +3916,11 @@
       <c r="D132" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E132" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E132" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>5</v>
       </c>
@@ -3947,11 +3933,11 @@
       <c r="D133" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E133" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E133" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>5</v>
       </c>
@@ -3964,11 +3950,11 @@
       <c r="D134" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E134" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E134" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>5</v>
       </c>
@@ -3981,11 +3967,11 @@
       <c r="D135" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E135" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E135" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>5</v>
       </c>
@@ -3998,11 +3984,11 @@
       <c r="D136" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E136" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E136" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>5</v>
       </c>
@@ -4015,11 +4001,11 @@
       <c r="D137" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E137" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E137" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>5</v>
       </c>
@@ -4032,11 +4018,11 @@
       <c r="D138" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E138" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E138" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>5</v>
       </c>
@@ -4049,11 +4035,11 @@
       <c r="D139" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E139" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="125.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E139" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="114.5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>5</v>
       </c>
@@ -4066,11 +4052,11 @@
       <c r="D140" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E140" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="189.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E140" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="137.5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>5</v>
       </c>
@@ -4083,11 +4069,11 @@
       <c r="D141" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E141" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E141" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>5</v>
       </c>
@@ -4100,11 +4086,11 @@
       <c r="D142" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E142" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E142" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>5</v>
       </c>
@@ -4117,11 +4103,11 @@
       <c r="D143" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E143" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E143" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>5</v>
       </c>
@@ -4134,11 +4120,11 @@
       <c r="D144" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E144" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E144" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="162.5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>5</v>
       </c>
@@ -4151,11 +4137,11 @@
       <c r="D145" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E145" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="178.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E145" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>5</v>
       </c>
@@ -4168,11 +4154,11 @@
       <c r="D146" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E146" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E146" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>5</v>
       </c>
@@ -4185,11 +4171,11 @@
       <c r="D147" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E147" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E147" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>5</v>
       </c>
@@ -4202,11 +4188,11 @@
       <c r="D148" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E148" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="156.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E148" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>5</v>
       </c>
@@ -4219,11 +4205,11 @@
       <c r="D149" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E149" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E149" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>5</v>
       </c>
@@ -4236,11 +4222,11 @@
       <c r="D150" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E150" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E150" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>5</v>
       </c>
@@ -4253,11 +4239,11 @@
       <c r="D151" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E151" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E151" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>5</v>
       </c>
@@ -4270,11 +4256,11 @@
       <c r="D152" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E152" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E152" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>5</v>
       </c>
@@ -4287,11 +4273,11 @@
       <c r="D153" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E153" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E153" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>5</v>
       </c>
@@ -4304,11 +4290,11 @@
       <c r="D154" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E154" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E154" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>5</v>
       </c>
@@ -4321,11 +4307,11 @@
       <c r="D155" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E155" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="167.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E155" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>5</v>
       </c>
@@ -4338,11 +4324,11 @@
       <c r="D156" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E156" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E156" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>5</v>
       </c>
@@ -4355,11 +4341,11 @@
       <c r="D157" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E157" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E157" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>5</v>
       </c>
@@ -4372,11 +4358,11 @@
       <c r="D158" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E158" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E158" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>5</v>
       </c>
@@ -4389,11 +4375,11 @@
       <c r="D159" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E159" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="156.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E159" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>5</v>
       </c>
@@ -4406,11 +4392,11 @@
       <c r="D160" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E160" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E160" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="187.5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>5</v>
       </c>
@@ -4423,11 +4409,11 @@
       <c r="D161" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E161" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E161" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>5</v>
       </c>
@@ -4440,11 +4426,11 @@
       <c r="D162" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E162" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E162" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>5</v>
       </c>
@@ -4457,11 +4443,11 @@
       <c r="D163" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E163" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E163" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>5</v>
       </c>
@@ -4474,11 +4460,11 @@
       <c r="D164" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E164" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E164" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="162.5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>5</v>
       </c>
@@ -4491,11 +4477,11 @@
       <c r="D165" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E165" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="178.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E165" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>5</v>
       </c>
@@ -4508,11 +4494,11 @@
       <c r="D166" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E166" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E166" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>5</v>
       </c>
@@ -4525,11 +4511,11 @@
       <c r="D167" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E167" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E167" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>5</v>
       </c>
@@ -4542,11 +4528,11 @@
       <c r="D168" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E168" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="167.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E168" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>5</v>
       </c>
@@ -4559,11 +4545,11 @@
       <c r="D169" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E169" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="134.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E169" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>5</v>
       </c>
@@ -4576,11 +4562,11 @@
       <c r="D170" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E170" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E170" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>5</v>
       </c>
@@ -4593,11 +4579,11 @@
       <c r="D171" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E171" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E171" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>5</v>
       </c>
@@ -4610,11 +4596,11 @@
       <c r="D172" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E172" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="156.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E172" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" ht="125" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>5</v>
       </c>
@@ -4627,11 +4613,11 @@
       <c r="D173" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E173" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E173" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>5</v>
       </c>
@@ -4644,11 +4630,11 @@
       <c r="D174" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E174" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E174" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>5</v>
       </c>
@@ -4661,11 +4647,11 @@
       <c r="D175" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E175" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="167.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E175" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>5</v>
       </c>
@@ -4678,11 +4664,11 @@
       <c r="D176" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E176" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E176" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>5</v>
       </c>
@@ -4695,11 +4681,11 @@
       <c r="D177" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E177" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E177" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>5</v>
       </c>
@@ -4712,11 +4698,11 @@
       <c r="D178" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E178" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E178" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="100" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>5</v>
       </c>
@@ -4729,11 +4715,11 @@
       <c r="D179" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E179" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="156.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E179" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>5</v>
       </c>
@@ -4746,11 +4732,11 @@
       <c r="D180" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E180" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E180" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="187.5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>5</v>
       </c>
@@ -4763,11 +4749,11 @@
       <c r="D181" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E181" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E181" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>5</v>
       </c>
@@ -4780,11 +4766,11 @@
       <c r="D182" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E182" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E182" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>5</v>
       </c>
@@ -4797,32 +4783,31 @@
       <c r="D183" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E183" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D184" s="1" t="s">
+      <c r="E183" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D184" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E184" s="1" t="n">
-        <f aca="false">SUM(E2:E183)</f>
+      <c r="E184" s="2">
+        <f>SUM(E2:E183)</f>
         <v>60</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D185" s="1" t="s">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D185" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E185" s="2" t="n">
-        <v>0.3297</v>
+      <c r="E185" s="3">
+        <v>0.32969999999999999</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>

</xml_diff>